<commit_message>
made minor changes to the OBC and BB
</commit_message>
<xml_diff>
--- a/hardware/Eagle Designs/BBB_OBC v3 /BOM (OBC v3).xlsx
+++ b/hardware/Eagle Designs/BBB_OBC v3 /BOM (OBC v3).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="217">
   <si>
     <t>Part</t>
   </si>
@@ -364,13 +364,7 @@
     <t>J2</t>
   </si>
   <si>
-    <t>J3</t>
-  </si>
-  <si>
     <t>J6</t>
-  </si>
-  <si>
-    <t>J7</t>
   </si>
   <si>
     <t>J9</t>
@@ -1527,115 +1521,115 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="P13" s="2" t="s">
+      <c r="P13" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="S13" s="1" t="s">
         <v>95</v>
       </c>
       <c r="T13" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="V13" s="2" t="s">
+      <c r="V13" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="W13" s="2" t="s">
+      <c r="W13" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="X13" s="2" t="s">
+      <c r="X13" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="Y13" s="2" t="s">
+      <c r="Y13" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="Z13" s="2" t="s">
+      <c r="Z13" s="1" t="s">
         <v>101</v>
       </c>
       <c r="AA13" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="AB13" s="2" t="s">
+      <c r="AB13" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AE13" s="2" t="s">
+      <c r="AE13" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AI13" s="2" t="s">
+      <c r="AI13" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AK13" s="2" t="s">
+      <c r="AK13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="AL13" s="2" t="s">
+      <c r="AL13" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AM13" s="2">
+      <c r="AM13" s="1">
         <v>0.0</v>
       </c>
-      <c r="AN13" s="2">
+      <c r="AN13" s="1">
         <v>0.0</v>
       </c>
-      <c r="AQ13" s="2" t="s">
+      <c r="AQ13" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AS13" s="2" t="s">
+      <c r="AS13" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AT13" s="2">
+      <c r="AT13" s="1">
         <v>4.0</v>
       </c>
-      <c r="AU13" s="2">
+      <c r="AU13" s="1">
         <v>1.0</v>
       </c>
-      <c r="AX13" s="2" t="s">
+      <c r="AX13" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BA13" s="2" t="s">
+      <c r="BA13" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="BC13" s="2" t="s">
+      <c r="BC13" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="BF13" s="2" t="s">
+      <c r="BF13" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="BH13" s="2" t="s">
+      <c r="BH13" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="BI13" s="2" t="s">
+      <c r="BI13" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BM13" s="2" t="s">
+      <c r="BM13" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="BN13" s="2" t="s">
+      <c r="BN13" s="1" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1644,455 +1638,317 @@
         <v>118</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="S14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA14" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB14" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE14" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AI14" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK14" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AL14" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AM14" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="AN14" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="AQ14" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AS14" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AT14" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="AU14" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="AX14" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BA14" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BC14" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BF14" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BH14" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BI14" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BM14" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BN14" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BG14" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BL14" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="S15" s="1" t="s">
-        <v>95</v>
+        <v>127</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="T15" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="X15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA15" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB15" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AE15" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AI15" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AK15" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AL15" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AM15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="AN15" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="AQ15" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AS15" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AT15" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="AU15" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="AX15" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BA15" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BC15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BF15" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BH15" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BI15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="BM15" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="BN15" s="1" t="s">
-        <v>115</v>
+        <v>129</v>
+      </c>
+      <c r="AJ15" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="BG15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BL15" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="R16" s="1" t="s">
-        <v>124</v>
+      <c r="T16" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="AJ16" s="1" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="BG16" s="1" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="BL16" s="1" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="R17" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="T17" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG17" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="BL17" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="AJ17" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="BG17" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BL17" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>124</v>
+        <v>140</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="T18" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="AJ18" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="BG18" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="BL18" s="1" t="s">
-        <v>133</v>
+        <v>142</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AQ18" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AS18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX18" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BC18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BF18" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="BH18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BI18" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="R19" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="BG19" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="BL19" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="T19" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ19" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="BG19" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="BL19" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>141</v>
+        <v>150</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>91</v>
+        <v>154</v>
       </c>
       <c r="T20" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y20" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z20" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI20" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AK20" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AQ20" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AS20" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AX20" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="BC20" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BF20" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="BH20" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BI20" s="1" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="AJ21" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="BG21" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="BL21" s="1" t="s">
-        <v>126</v>
+        <v>140</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AQ21" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AS21" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AX21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BC21" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BF21" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="BH21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BI21" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>156</v>
+        <v>135</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="T22" s="3" t="s">
-        <v>157</v>
+        <v>136</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG22" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="BL22" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="23">
@@ -2100,55 +1956,31 @@
         <v>158</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>91</v>
+        <v>135</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="T23" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="Y23" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Z23" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI23" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AK23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AQ23" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AS23" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="AX23" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="BC23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BF23" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="BH23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BI23" s="1" t="s">
-        <v>113</v>
+        <v>136</v>
+      </c>
+      <c r="AJ23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG23" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="BL23" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="24">
@@ -2156,344 +1988,280 @@
         <v>159</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="T24" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ24" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="BG24" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="BL24" s="1" t="s">
-        <v>133</v>
+        <v>160</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK24" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AS24" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV24" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AW24" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="C25" s="1" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="T25" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="BG25" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="BL25" s="1" t="s">
-        <v>133</v>
+        <v>160</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AK25" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AS25" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AV25" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AW25" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
+      </c>
+      <c r="D26" s="1">
+        <v>805.0</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="AK26" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="AS26" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AV26" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AW26" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>162</v>
+        <v>168</v>
+      </c>
+      <c r="D27" s="1">
+        <v>805.0</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="AK27" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="AS27" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AV27" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AW27" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="D28" s="1">
         <v>805.0</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D29" s="1">
-        <v>805.0</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ29" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="AO29" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" s="1">
-        <v>805.0</v>
+        <v>181</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>171</v>
+        <v>183</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1432281.0</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="T30" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC30" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD30" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF30" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG30" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH30" s="1">
+        <v>1.521843574E9</v>
+      </c>
+      <c r="AK30" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AP30" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AS30" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AX30" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="AY30" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="AZ30" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="BC30" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="BE30" s="1">
+        <v>1.377817843E9</v>
+      </c>
+      <c r="BF30" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BJ30" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="BK30" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>177</v>
+        <v>203</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="AJ31" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AO31" s="1" t="s">
-        <v>181</v>
+        <v>203</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AK31" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AR31" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX31" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="BD31" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>183</v>
+        <v>212</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="J32" s="1">
-        <v>1432281.0</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="L32" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="N32" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="T32" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="AB32" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="AC32" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="AD32" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="AF32" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AG32" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="AH32" s="1">
-        <v>1.521843574E9</v>
-      </c>
-      <c r="AK32" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="AP32" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AS32" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX32" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="AY32" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="AZ32" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="BC32" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="BE32" s="1">
-        <v>1.377817843E9</v>
-      </c>
-      <c r="BF32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BJ32" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="BK32" s="1" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="U33" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="AK33" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="AR33" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="AX33" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="BD33" s="1" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2506,22 +2274,18 @@
     <hyperlink r:id="rId6" ref="AA12"/>
     <hyperlink r:id="rId7" ref="T13"/>
     <hyperlink r:id="rId8" ref="AA13"/>
-    <hyperlink r:id="rId9" ref="T14"/>
-    <hyperlink r:id="rId10" ref="AA14"/>
-    <hyperlink r:id="rId11" ref="T15"/>
-    <hyperlink r:id="rId12" ref="AA15"/>
-    <hyperlink r:id="rId13" ref="T17"/>
-    <hyperlink r:id="rId14" ref="T18"/>
-    <hyperlink r:id="rId15" ref="T19"/>
-    <hyperlink r:id="rId16" ref="T20"/>
-    <hyperlink r:id="rId17" ref="T22"/>
-    <hyperlink r:id="rId18" ref="T23"/>
-    <hyperlink r:id="rId19" ref="T24"/>
-    <hyperlink r:id="rId20" ref="T25"/>
-    <hyperlink r:id="rId21" ref="L32"/>
-    <hyperlink r:id="rId22" ref="N32"/>
-    <hyperlink r:id="rId23" ref="T32"/>
+    <hyperlink r:id="rId9" ref="T15"/>
+    <hyperlink r:id="rId10" ref="T16"/>
+    <hyperlink r:id="rId11" ref="T17"/>
+    <hyperlink r:id="rId12" ref="T18"/>
+    <hyperlink r:id="rId13" ref="T20"/>
+    <hyperlink r:id="rId14" ref="T21"/>
+    <hyperlink r:id="rId15" ref="T22"/>
+    <hyperlink r:id="rId16" ref="T23"/>
+    <hyperlink r:id="rId17" ref="L30"/>
+    <hyperlink r:id="rId18" ref="N30"/>
+    <hyperlink r:id="rId19" ref="T30"/>
   </hyperlinks>
-  <drawing r:id="rId24"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>